<commit_message>
adding incident tables ferry and klickitat
</commit_message>
<xml_diff>
--- a/County-SO-Data/Ferry/Ferry.xlsx
+++ b/County-SO-Data/Ferry/Ferry.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidris\Documents\GitHub\wa-pursuit-pdr-data\County-SO-Data\Ferry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E5D742F-019D-479A-B6D4-93AF5D16862F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBC57AD-495C-4B42-B56A-CBD2B17B0C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="1430" windowWidth="14400" windowHeight="7360" xr2:uid="{F1AB79A4-CB9C-4588-ABFE-9AD08FB423BF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F1AB79A4-CB9C-4588-ABFE-9AD08FB423BF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Table" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,12 +37,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
   <si>
     <t>Year</t>
   </si>
   <si>
     <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Month</t>
   </si>
 </sst>
 </file>
@@ -439,11 +443,82 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F3BF75A-D79E-46F6-A771-623BA7E4C16C}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>2023</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4C3B4D-D5A0-4EE7-8572-A5AE975B6E7F}">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView zoomScale="83" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
update scrape and excel for Ferry Co SO
</commit_message>
<xml_diff>
--- a/County-SO-Data/Ferry/Ferry.xlsx
+++ b/County-SO-Data/Ferry/Ferry.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidris\Documents\GitHub\wa-pursuit-pdr-data\County-SO-Data\Ferry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Documents\GitHub\wa-pursuit-pdr-data\County-SO-Data\Ferry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526B779B-0EE3-4A6E-811E-BBAC66B057F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04165CD3-420C-46D6-93EA-1577335425EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F1AB79A4-CB9C-4588-ABFE-9AD08FB423BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F1AB79A4-CB9C-4588-ABFE-9AD08FB423BF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Incidents" sheetId="2" r:id="rId1"/>
     <sheet name="Table" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -448,9 +448,9 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -458,7 +458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11</v>
       </c>
@@ -466,7 +466,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -474,7 +474,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>8</v>
       </c>
@@ -482,7 +482,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -490,7 +490,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>8</v>
       </c>
@@ -498,7 +498,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>8</v>
       </c>
@@ -516,12 +516,12 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView zoomScale="83" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -565,7 +565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>2019</v>
       </c>
@@ -588,7 +588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2020</v>
       </c>
@@ -613,7 +613,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2021</v>
       </c>
@@ -636,7 +636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>2022</v>
       </c>
@@ -659,7 +659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>2023</v>
       </c>
@@ -682,7 +682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>

</xml_diff>